<commit_message>
updates and data cleaning
</commit_message>
<xml_diff>
--- a/tools/temp/papers-out.xlsx
+++ b/tools/temp/papers-out.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\sample-pages\tools\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D181A95E-A255-45B3-BCA7-DBBCBF3F8620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF9A057-BE4C-48EA-82C7-1894FF13C42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="3495" windowWidth="28800" windowHeight="17145" xr2:uid="{E6338481-C6B1-405C-BD98-5DBA4A89B2D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{969D0237-402E-4DC4-B970-00B4EB701D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="papers-out" sheetId="1" r:id="rId1"/>
@@ -2208,12 +2208,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AFB607-31EB-45D9-BF79-03AA1408D5DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F180D6-F288-4798-B7D4-4E758C77F56C}">
   <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3979,4 +3982,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>